<commit_message>
Storing faculty name in FacultyCell
</commit_message>
<xml_diff>
--- a/programInfo/KCP.xlsx
+++ b/programInfo/KCP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Qt\ApplicantStatsProject\programInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4189718-DC0B-4624-BB27-6235FC22194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDCEE55-6CF3-4978-98F0-DB40A15B4132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5590EB21-9F4B-4755-A428-4D332FCC201A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5590EB21-9F4B-4755-A428-4D332FCC201A}"/>
   </bookViews>
   <sheets>
     <sheet name="Бакалавры" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="103">
   <si>
     <t>Медицинская и фармацевтическая химия</t>
   </si>
@@ -581,7 +581,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -589,12 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -614,23 +620,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,13 +974,13 @@
   <dimension ref="A1:R169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
@@ -992,7 +992,7 @@
       <c r="A1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="16" t="s">
         <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1010,13 +1010,13 @@
       <c r="G1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -1028,7 +1028,7 @@
       <c r="A2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1063,7 +1063,9 @@
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1078,11 +1080,11 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
@@ -1095,7 +1097,9 @@
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1129,9 @@
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1140,11 +1146,11 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
@@ -1162,7 +1168,7 @@
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -1179,7 +1185,7 @@
       <c r="A7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1199,24 +1205,26 @@
         <v>19</v>
       </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
       <c r="R7" s="13"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1231,24 +1239,26 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
       <c r="R8" s="13"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1263,24 +1273,26 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
       <c r="R9" s="13"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1295,16 +1307,16 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="13"/>
     </row>
@@ -1317,7 +1329,7 @@
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="12"/>
       <c r="I11" s="11" t="s">
         <v>81</v>
@@ -1336,7 +1348,7 @@
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1356,24 +1368,26 @@
         <v>15</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
       <c r="R12" s="13"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1388,24 +1402,26 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1453,9 @@
       <c r="A15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="30"/>
+      <c r="B15" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1452,17 +1470,17 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
       <c r="R15" s="13"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -1474,7 +1492,7 @@
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -1491,7 +1509,7 @@
       <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="30" t="s">
         <v>93</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1515,7 +1533,9 @@
       <c r="A18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +1554,9 @@
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1575,9 @@
       <c r="A20" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
@@ -1569,21 +1593,21 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1607,7 +1631,9 @@
       <c r="A23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -1626,7 +1652,9 @@
       <c r="A24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1673,9 @@
       <c r="A25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="30"/>
+      <c r="B25" s="32" t="s">
+        <v>94</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
@@ -1661,21 +1691,21 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1699,7 +1729,9 @@
       <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1750,9 @@
       <c r="A29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
@@ -1737,7 +1771,9 @@
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="30"/>
+      <c r="B30" s="32" t="s">
+        <v>94</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1753,21 +1789,21 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1791,7 +1827,9 @@
       <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
@@ -1810,7 +1848,9 @@
       <c r="A34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="29"/>
+      <c r="B34" s="31" t="s">
+        <v>94</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1829,7 +1869,9 @@
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="30"/>
+      <c r="B35" s="32" t="s">
+        <v>94</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>11</v>
       </c>
@@ -1845,21 +1887,21 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="30" t="s">
         <v>95</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1883,7 +1925,9 @@
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="29"/>
+      <c r="B38" s="31" t="s">
+        <v>95</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>13</v>
       </c>
@@ -1902,7 +1946,9 @@
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="29"/>
+      <c r="B39" s="31" t="s">
+        <v>95</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>13</v>
       </c>
@@ -1921,7 +1967,9 @@
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="30"/>
+      <c r="B40" s="32" t="s">
+        <v>95</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>13</v>
       </c>
@@ -1937,21 +1985,21 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="30" t="s">
         <v>95</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1975,7 +2023,9 @@
       <c r="A43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="29"/>
+      <c r="B43" s="31" t="s">
+        <v>95</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +2044,9 @@
       <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="29"/>
+      <c r="B44" s="31" t="s">
+        <v>95</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2065,9 @@
       <c r="A45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="30"/>
+      <c r="B45" s="32" t="s">
+        <v>95</v>
+      </c>
       <c r="C45" s="4" t="s">
         <v>15</v>
       </c>
@@ -2029,21 +2083,21 @@
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -2067,7 +2121,9 @@
       <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="29"/>
+      <c r="B48" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C48" s="4" t="s">
         <v>16</v>
       </c>
@@ -2086,7 +2142,9 @@
       <c r="A49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="29"/>
+      <c r="B49" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>16</v>
       </c>
@@ -2105,7 +2163,9 @@
       <c r="A50" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="30"/>
+      <c r="B50" s="32" t="s">
+        <v>96</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>16</v>
       </c>
@@ -2121,21 +2181,21 @@
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -2159,7 +2219,9 @@
       <c r="A53" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="29"/>
+      <c r="B53" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>17</v>
       </c>
@@ -2178,7 +2240,9 @@
       <c r="A54" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="29"/>
+      <c r="B54" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C54" s="4" t="s">
         <v>17</v>
       </c>
@@ -2197,7 +2261,9 @@
       <c r="A55" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="30"/>
+      <c r="B55" s="32" t="s">
+        <v>96</v>
+      </c>
       <c r="C55" s="4" t="s">
         <v>17</v>
       </c>
@@ -2213,21 +2279,21 @@
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -2251,7 +2317,9 @@
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C58" s="4" t="s">
         <v>18</v>
       </c>
@@ -2270,7 +2338,9 @@
       <c r="A59" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="29"/>
+      <c r="B59" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C59" s="4" t="s">
         <v>18</v>
       </c>
@@ -2289,7 +2359,9 @@
       <c r="A60" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="30"/>
+      <c r="B60" s="32" t="s">
+        <v>96</v>
+      </c>
       <c r="C60" s="4" t="s">
         <v>18</v>
       </c>
@@ -2305,21 +2377,21 @@
       <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="30" t="s">
         <v>96</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -2343,7 +2415,9 @@
       <c r="A63" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="29"/>
+      <c r="B63" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C63" s="4" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2436,9 @@
       <c r="A64" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="31" t="s">
+        <v>96</v>
+      </c>
       <c r="C64" s="4" t="s">
         <v>19</v>
       </c>
@@ -2381,7 +2457,9 @@
       <c r="A65" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="30"/>
+      <c r="B65" s="32" t="s">
+        <v>96</v>
+      </c>
       <c r="C65" s="4" t="s">
         <v>19</v>
       </c>
@@ -2397,21 +2475,21 @@
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="30" t="s">
         <v>97</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -2435,7 +2513,9 @@
       <c r="A68" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B68" s="29"/>
+      <c r="B68" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="C68" s="4" t="s">
         <v>21</v>
       </c>
@@ -2454,7 +2534,9 @@
       <c r="A69" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B69" s="29"/>
+      <c r="B69" s="31" t="s">
+        <v>97</v>
+      </c>
       <c r="C69" s="4" t="s">
         <v>21</v>
       </c>
@@ -2473,7 +2555,9 @@
       <c r="A70" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B70" s="30"/>
+      <c r="B70" s="32" t="s">
+        <v>97</v>
+      </c>
       <c r="C70" s="4" t="s">
         <v>21</v>
       </c>
@@ -2489,21 +2573,21 @@
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="30" t="s">
         <v>98</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -2527,7 +2611,9 @@
       <c r="A73" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="29"/>
+      <c r="B73" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C73" s="4" t="s">
         <v>23</v>
       </c>
@@ -2546,7 +2632,9 @@
       <c r="A74" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="29"/>
+      <c r="B74" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C74" s="4" t="s">
         <v>23</v>
       </c>
@@ -2565,7 +2653,9 @@
       <c r="A75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="29"/>
+      <c r="B75" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C75" s="4" t="s">
         <v>24</v>
       </c>
@@ -2584,7 +2674,9 @@
       <c r="A76" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B76" s="30"/>
+      <c r="B76" s="32" t="s">
+        <v>98</v>
+      </c>
       <c r="C76" s="4" t="s">
         <v>25</v>
       </c>
@@ -2600,21 +2692,21 @@
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="30" t="s">
         <v>98</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -2638,7 +2730,9 @@
       <c r="A79" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="29"/>
+      <c r="B79" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C79" s="4" t="s">
         <v>27</v>
       </c>
@@ -2657,7 +2751,9 @@
       <c r="A80" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B80" s="29"/>
+      <c r="B80" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C80" s="4" t="s">
         <v>27</v>
       </c>
@@ -2676,7 +2772,9 @@
       <c r="A81" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B81" s="29"/>
+      <c r="B81" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C81" s="4" t="s">
         <v>28</v>
       </c>
@@ -2695,7 +2793,9 @@
       <c r="A82" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B82" s="29"/>
+      <c r="B82" s="31" t="s">
+        <v>98</v>
+      </c>
       <c r="C82" s="4" t="s">
         <v>29</v>
       </c>
@@ -2714,7 +2814,9 @@
       <c r="A83" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B83" s="30"/>
+      <c r="B83" s="32" t="s">
+        <v>98</v>
+      </c>
       <c r="C83" s="4" t="s">
         <v>30</v>
       </c>
@@ -2730,21 +2832,21 @@
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B85" s="28" t="s">
+      <c r="B85" s="30" t="s">
         <v>99</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -2768,7 +2870,9 @@
       <c r="A86" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B86" s="29"/>
+      <c r="B86" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C86" s="4" t="s">
         <v>32</v>
       </c>
@@ -2787,7 +2891,9 @@
       <c r="A87" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B87" s="29"/>
+      <c r="B87" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C87" s="4" t="s">
         <v>32</v>
       </c>
@@ -2806,7 +2912,9 @@
       <c r="A88" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="30"/>
+      <c r="B88" s="32" t="s">
+        <v>99</v>
+      </c>
       <c r="C88" s="4" t="s">
         <v>32</v>
       </c>
@@ -2822,21 +2930,21 @@
       <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
+      <c r="A89" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="21"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="B90" s="30" t="s">
         <v>99</v>
       </c>
       <c r="C90" s="4" t="s">
@@ -2860,7 +2968,9 @@
       <c r="A91" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B91" s="29"/>
+      <c r="B91" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C91" s="4" t="s">
         <v>34</v>
       </c>
@@ -2879,7 +2989,9 @@
       <c r="A92" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="29"/>
+      <c r="B92" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C92" s="4" t="s">
         <v>34</v>
       </c>
@@ -2898,7 +3010,9 @@
       <c r="A93" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="30"/>
+      <c r="B93" s="32" t="s">
+        <v>99</v>
+      </c>
       <c r="C93" s="4" t="s">
         <v>34</v>
       </c>
@@ -2914,21 +3028,21 @@
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+      <c r="A94" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="28" t="s">
+      <c r="B95" s="30" t="s">
         <v>99</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -2952,7 +3066,9 @@
       <c r="A96" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B96" s="29"/>
+      <c r="B96" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C96" s="4" t="s">
         <v>35</v>
       </c>
@@ -2971,7 +3087,9 @@
       <c r="A97" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B97" s="29"/>
+      <c r="B97" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="C97" s="4" t="s">
         <v>35</v>
       </c>
@@ -2990,7 +3108,9 @@
       <c r="A98" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B98" s="30"/>
+      <c r="B98" s="32" t="s">
+        <v>99</v>
+      </c>
       <c r="C98" s="4" t="s">
         <v>35</v>
       </c>
@@ -3006,21 +3126,21 @@
       <c r="G98" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+      <c r="A99" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B100" s="28" t="s">
+      <c r="B100" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -3044,7 +3164,9 @@
       <c r="A101" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B101" s="29"/>
+      <c r="B101" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C101" s="4" t="s">
         <v>37</v>
       </c>
@@ -3063,7 +3185,9 @@
       <c r="A102" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="29"/>
+      <c r="B102" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C102" s="4" t="s">
         <v>37</v>
       </c>
@@ -3082,7 +3206,9 @@
       <c r="A103" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B103" s="30"/>
+      <c r="B103" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C103" s="4" t="s">
         <v>37</v>
       </c>
@@ -3098,21 +3224,21 @@
       <c r="G103" s="3"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+      <c r="A104" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="17"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B105" s="28" t="s">
+      <c r="B105" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C105" s="4" t="s">
@@ -3136,7 +3262,9 @@
       <c r="A106" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B106" s="29"/>
+      <c r="B106" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C106" s="4" t="s">
         <v>39</v>
       </c>
@@ -3155,7 +3283,9 @@
       <c r="A107" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B107" s="29"/>
+      <c r="B107" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C107" s="4" t="s">
         <v>39</v>
       </c>
@@ -3174,7 +3304,9 @@
       <c r="A108" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B108" s="30"/>
+      <c r="B108" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C108" s="4" t="s">
         <v>39</v>
       </c>
@@ -3190,21 +3322,21 @@
       <c r="G108" s="3"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+      <c r="A109" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="17"/>
-      <c r="G109" s="17"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B110" s="28" t="s">
+      <c r="B110" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C110" s="4" t="s">
@@ -3228,7 +3360,9 @@
       <c r="A111" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B111" s="29"/>
+      <c r="B111" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C111" s="4" t="s">
         <v>41</v>
       </c>
@@ -3247,7 +3381,9 @@
       <c r="A112" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B112" s="29"/>
+      <c r="B112" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C112" s="4" t="s">
         <v>41</v>
       </c>
@@ -3266,7 +3402,9 @@
       <c r="A113" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B113" s="30"/>
+      <c r="B113" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C113" s="4" t="s">
         <v>41</v>
       </c>
@@ -3282,21 +3420,21 @@
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="16" t="s">
+      <c r="A114" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="21"/>
+      <c r="G114" s="21"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B115" s="28" t="s">
+      <c r="B115" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C115" s="4" t="s">
@@ -3320,7 +3458,9 @@
       <c r="A116" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B116" s="29"/>
+      <c r="B116" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C116" s="4" t="s">
         <v>41</v>
       </c>
@@ -3339,7 +3479,9 @@
       <c r="A117" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B117" s="29"/>
+      <c r="B117" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C117" s="4" t="s">
         <v>41</v>
       </c>
@@ -3358,7 +3500,9 @@
       <c r="A118" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B118" s="30"/>
+      <c r="B118" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C118" s="4" t="s">
         <v>41</v>
       </c>
@@ -3374,21 +3518,21 @@
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
+      <c r="A119" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="17"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="21"/>
+      <c r="D119" s="21"/>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="21"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B120" s="28" t="s">
+      <c r="B120" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C120" s="4" t="s">
@@ -3412,7 +3556,9 @@
       <c r="A121" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B121" s="29"/>
+      <c r="B121" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C121" s="4" t="s">
         <v>44</v>
       </c>
@@ -3431,7 +3577,9 @@
       <c r="A122" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B122" s="29"/>
+      <c r="B122" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C122" s="4" t="s">
         <v>44</v>
       </c>
@@ -3450,7 +3598,9 @@
       <c r="A123" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B123" s="30"/>
+      <c r="B123" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C123" s="4" t="s">
         <v>44</v>
       </c>
@@ -3466,21 +3616,21 @@
       <c r="G123" s="3"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+      <c r="A124" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B124" s="17"/>
-      <c r="C124" s="17"/>
-      <c r="D124" s="17"/>
-      <c r="E124" s="17"/>
-      <c r="F124" s="17"/>
-      <c r="G124" s="17"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="21"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B125" s="28" t="s">
+      <c r="B125" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C125" s="4" t="s">
@@ -3504,7 +3654,9 @@
       <c r="A126" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B126" s="29"/>
+      <c r="B126" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C126" s="4" t="s">
         <v>46</v>
       </c>
@@ -3523,7 +3675,9 @@
       <c r="A127" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B127" s="29"/>
+      <c r="B127" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="C127" s="4" t="s">
         <v>46</v>
       </c>
@@ -3542,7 +3696,9 @@
       <c r="A128" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B128" s="30"/>
+      <c r="B128" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="C128" s="4" t="s">
         <v>46</v>
       </c>
@@ -3558,21 +3714,21 @@
       <c r="G128" s="3"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
+      <c r="A129" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B129" s="17"/>
-      <c r="C129" s="17"/>
-      <c r="D129" s="17"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="17"/>
-      <c r="G129" s="17"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="21"/>
+      <c r="E129" s="21"/>
+      <c r="F129" s="21"/>
+      <c r="G129" s="21"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="B130" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C130" s="4" t="s">
@@ -3596,7 +3752,9 @@
       <c r="A131" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B131" s="29"/>
+      <c r="B131" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C131" s="4" t="s">
         <v>48</v>
       </c>
@@ -3615,7 +3773,9 @@
       <c r="A132" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B132" s="29"/>
+      <c r="B132" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C132" s="4" t="s">
         <v>48</v>
       </c>
@@ -3634,7 +3794,9 @@
       <c r="A133" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B133" s="30"/>
+      <c r="B133" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C133" s="4" t="s">
         <v>48</v>
       </c>
@@ -3650,21 +3812,21 @@
       <c r="G133" s="3"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+      <c r="A134" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B134" s="17"/>
-      <c r="C134" s="17"/>
-      <c r="D134" s="17"/>
-      <c r="E134" s="17"/>
-      <c r="F134" s="17"/>
-      <c r="G134" s="17"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="21"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="21"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B135" s="28" t="s">
+      <c r="B135" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C135" s="4" t="s">
@@ -3688,7 +3850,9 @@
       <c r="A136" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B136" s="29"/>
+      <c r="B136" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C136" s="4" t="s">
         <v>49</v>
       </c>
@@ -3707,7 +3871,9 @@
       <c r="A137" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B137" s="29"/>
+      <c r="B137" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C137" s="4" t="s">
         <v>49</v>
       </c>
@@ -3726,7 +3892,9 @@
       <c r="A138" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B138" s="30"/>
+      <c r="B138" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C138" s="4" t="s">
         <v>49</v>
       </c>
@@ -3742,21 +3910,21 @@
       <c r="G138" s="3"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
+      <c r="A139" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B139" s="17"/>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="17"/>
-      <c r="F139" s="17"/>
-      <c r="G139" s="17"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="21"/>
+      <c r="D139" s="21"/>
+      <c r="E139" s="21"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="21"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B140" s="28" t="s">
+      <c r="B140" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C140" s="4" t="s">
@@ -3780,7 +3948,9 @@
       <c r="A141" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B141" s="29"/>
+      <c r="B141" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C141" s="4" t="s">
         <v>50</v>
       </c>
@@ -3799,7 +3969,9 @@
       <c r="A142" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B142" s="29"/>
+      <c r="B142" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C142" s="4" t="s">
         <v>50</v>
       </c>
@@ -3818,7 +3990,9 @@
       <c r="A143" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B143" s="30"/>
+      <c r="B143" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C143" s="4" t="s">
         <v>50</v>
       </c>
@@ -3834,21 +4008,21 @@
       <c r="G143" s="3"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
+      <c r="A144" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B144" s="17"/>
-      <c r="C144" s="17"/>
-      <c r="D144" s="17"/>
-      <c r="E144" s="17"/>
-      <c r="F144" s="17"/>
-      <c r="G144" s="17"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="21"/>
+      <c r="E144" s="21"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="21"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B145" s="28" t="s">
+      <c r="B145" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C145" s="4" t="s">
@@ -3872,7 +4046,9 @@
       <c r="A146" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B146" s="29"/>
+      <c r="B146" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C146" s="4" t="s">
         <v>52</v>
       </c>
@@ -3891,7 +4067,9 @@
       <c r="A147" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B147" s="29"/>
+      <c r="B147" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C147" s="4" t="s">
         <v>52</v>
       </c>
@@ -3910,7 +4088,9 @@
       <c r="A148" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B148" s="30"/>
+      <c r="B148" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C148" s="4" t="s">
         <v>52</v>
       </c>
@@ -3926,21 +4106,21 @@
       <c r="G148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
+      <c r="A149" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B149" s="17"/>
-      <c r="C149" s="17"/>
-      <c r="D149" s="17"/>
-      <c r="E149" s="17"/>
-      <c r="F149" s="17"/>
-      <c r="G149" s="17"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="21"/>
+      <c r="E149" s="21"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="21"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B150" s="28" t="s">
+      <c r="B150" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C150" s="4" t="s">
@@ -3964,7 +4144,9 @@
       <c r="A151" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B151" s="29"/>
+      <c r="B151" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C151" s="4" t="s">
         <v>53</v>
       </c>
@@ -3983,7 +4165,9 @@
       <c r="A152" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B152" s="29"/>
+      <c r="B152" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C152" s="4" t="s">
         <v>53</v>
       </c>
@@ -4002,7 +4186,9 @@
       <c r="A153" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B153" s="30"/>
+      <c r="B153" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C153" s="4" t="s">
         <v>53</v>
       </c>
@@ -4018,21 +4204,21 @@
       <c r="G153" s="3"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
+      <c r="A154" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B154" s="17"/>
-      <c r="C154" s="17"/>
-      <c r="D154" s="17"/>
-      <c r="E154" s="17"/>
-      <c r="F154" s="17"/>
-      <c r="G154" s="17"/>
+      <c r="B154" s="21"/>
+      <c r="C154" s="21"/>
+      <c r="D154" s="21"/>
+      <c r="E154" s="21"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="21"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B155" s="28" t="s">
+      <c r="B155" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C155" s="4" t="s">
@@ -4056,7 +4242,9 @@
       <c r="A156" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B156" s="29"/>
+      <c r="B156" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C156" s="4" t="s">
         <v>55</v>
       </c>
@@ -4075,7 +4263,9 @@
       <c r="A157" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B157" s="29"/>
+      <c r="B157" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="C157" s="4" t="s">
         <v>55</v>
       </c>
@@ -4094,7 +4284,9 @@
       <c r="A158" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B158" s="30"/>
+      <c r="B158" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="C158" s="4" t="s">
         <v>55</v>
       </c>
@@ -4110,21 +4302,21 @@
       <c r="G158" s="3"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+      <c r="A159" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B159" s="17"/>
-      <c r="C159" s="17"/>
-      <c r="D159" s="17"/>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
-      <c r="G159" s="17"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="21"/>
+      <c r="E159" s="21"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="21"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B160" s="28" t="s">
+      <c r="B160" s="30" t="s">
         <v>102</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -4148,7 +4340,9 @@
       <c r="A161" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B161" s="29"/>
+      <c r="B161" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="C161" s="4" t="s">
         <v>57</v>
       </c>
@@ -4167,7 +4361,9 @@
       <c r="A162" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B162" s="29"/>
+      <c r="B162" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="C162" s="4" t="s">
         <v>57</v>
       </c>
@@ -4186,7 +4382,9 @@
       <c r="A163" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B163" s="30"/>
+      <c r="B163" s="32" t="s">
+        <v>102</v>
+      </c>
       <c r="C163" s="4" t="s">
         <v>57</v>
       </c>
@@ -4202,21 +4400,21 @@
       <c r="G163" s="3"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" s="16" t="s">
+      <c r="A164" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B164" s="17"/>
-      <c r="C164" s="17"/>
-      <c r="D164" s="17"/>
-      <c r="E164" s="17"/>
-      <c r="F164" s="17"/>
-      <c r="G164" s="17"/>
+      <c r="B164" s="21"/>
+      <c r="C164" s="21"/>
+      <c r="D164" s="21"/>
+      <c r="E164" s="21"/>
+      <c r="F164" s="21"/>
+      <c r="G164" s="21"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B165" s="28" t="s">
+      <c r="B165" s="30" t="s">
         <v>102</v>
       </c>
       <c r="C165" s="4" t="s">
@@ -4240,7 +4438,9 @@
       <c r="A166" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B166" s="29"/>
+      <c r="B166" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="C166" s="4" t="s">
         <v>57</v>
       </c>
@@ -4259,7 +4459,9 @@
       <c r="A167" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B167" s="29"/>
+      <c r="B167" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="C167" s="4" t="s">
         <v>57</v>
       </c>
@@ -4278,7 +4480,9 @@
       <c r="A168" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B168" s="30"/>
+      <c r="B168" s="32" t="s">
+        <v>102</v>
+      </c>
       <c r="C168" s="4" t="s">
         <v>57</v>
       </c>
@@ -4294,81 +4498,18 @@
       <c r="G168" s="3"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+      <c r="A169" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="B169" s="17"/>
-      <c r="C169" s="17"/>
-      <c r="D169" s="17"/>
-      <c r="E169" s="17"/>
-      <c r="F169" s="17"/>
-      <c r="G169" s="17"/>
+      <c r="B169" s="21"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="21"/>
+      <c r="E169" s="21"/>
+      <c r="F169" s="21"/>
+      <c r="G169" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B135:B138"/>
-    <mergeCell ref="B140:B143"/>
-    <mergeCell ref="B145:B148"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B78:B83"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="I10:P10"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="I12:Q12"/>
-    <mergeCell ref="I13:Q13"/>
-    <mergeCell ref="I15:Q15"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A134:G134"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A84:G84"/>
-    <mergeCell ref="A89:G89"/>
-    <mergeCell ref="A94:G94"/>
-    <mergeCell ref="A99:G99"/>
-    <mergeCell ref="A104:G104"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="B115:B118"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="B125:B128"/>
-    <mergeCell ref="B130:B133"/>
-    <mergeCell ref="A109:G109"/>
+  <mergeCells count="43">
     <mergeCell ref="A114:G114"/>
     <mergeCell ref="A119:G119"/>
     <mergeCell ref="A124:G124"/>
@@ -4380,8 +4521,38 @@
     <mergeCell ref="A154:G154"/>
     <mergeCell ref="A159:G159"/>
     <mergeCell ref="A164:G164"/>
-    <mergeCell ref="B160:B163"/>
-    <mergeCell ref="B165:B168"/>
+    <mergeCell ref="A134:G134"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="A89:G89"/>
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A99:G99"/>
+    <mergeCell ref="A104:G104"/>
+    <mergeCell ref="A109:G109"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="I12:Q12"/>
+    <mergeCell ref="I13:Q13"/>
+    <mergeCell ref="I15:Q15"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="I7:Q7"/>
+    <mergeCell ref="I10:P10"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="I9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>